<commit_message>
Toda parte da homologação feita
</commit_message>
<xml_diff>
--- a/documentacao/requisitos/testesHomologacao.xlsx
+++ b/documentacao/requisitos/testesHomologacao.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giuli\Desktop\grupo9-ads\documentacao\requisitos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vitória Cristina\Desktop\grupo9-ads\documentacao\requisitos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61A25FE5-6BC7-4F49-AA82-B6AEA538C4FA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B5FE85C-0BD5-4155-A490-F8D1218ADFAC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="503" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="503" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plano de Homologação" sheetId="5" r:id="rId1"/>
     <sheet name="Cenário 1 - Login" sheetId="6" r:id="rId2"/>
     <sheet name="Cenário 2 - Alertas" sheetId="7" r:id="rId3"/>
-    <sheet name="Regressão Básica" sheetId="4" r:id="rId4"/>
+    <sheet name="Cenário 3 - Gráficos" sheetId="8" r:id="rId4"/>
+    <sheet name="Regressão Básica" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
@@ -49,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="142">
   <si>
     <t xml:space="preserve">Projeto: </t>
   </si>
@@ -143,9 +144,6 @@
   </si>
   <si>
     <t>Codigo da demanda:</t>
-  </si>
-  <si>
-    <t>OK</t>
   </si>
   <si>
     <t>Pré-Requisitos:</t>
@@ -334,21 +332,12 @@
     <t>Entrar no Site</t>
   </si>
   <si>
-    <t>Entrar no site www.meuprojeto.com</t>
-  </si>
-  <si>
     <t>Login</t>
   </si>
   <si>
-    <t>Selecionar o menu Login</t>
-  </si>
-  <si>
     <t>Digitar um login/email válido</t>
   </si>
   <si>
-    <t>Digitar uma senha válida e clicar no botão ok/login</t>
-  </si>
-  <si>
     <t>Dashboard</t>
   </si>
   <si>
@@ -388,24 +377,15 @@
     <t>Abrir o site institucional do PharmaSensors, clicar na opção do menu 'login'; Inserir o email do usuário no campo e-mail; ir para o campo senha</t>
   </si>
   <si>
-    <t>Email do usuário =  pharma@teste.com</t>
-  </si>
-  <si>
     <t xml:space="preserve">Ser redirecionado para a tela do usuário </t>
   </si>
   <si>
     <t>RF-04-02</t>
   </si>
   <si>
-    <t>Email do usuário =  pharmaerro@gmail.com</t>
-  </si>
-  <si>
     <t>Abrir o site institucional do PharmaSensors, clicar na opção do menu 'login'; não inserir o email do usuário no campo e-mail; ir para o campo senha</t>
   </si>
   <si>
-    <t>Exibir a mensagem de erro "Favor preencher campos!"; voltar para campo Login</t>
-  </si>
-  <si>
     <t>RF-04-03</t>
   </si>
   <si>
@@ -421,9 +401,6 @@
     <t>Clicar na opção 'esqueci a senha'; é redirecionado a tela correspondente; Colocar nome e e-mail; Preencher Mensagem</t>
   </si>
   <si>
-    <t>Email do cliente = pharma@teste.com</t>
-  </si>
-  <si>
     <t>O sistema deve enviar um Email ao administrador com a mensagem do cliente.</t>
   </si>
   <si>
@@ -448,9 +425,6 @@
     <t>Atingiu o esperado</t>
   </si>
   <si>
-    <t>Fernando Maia, Giulia Maia</t>
-  </si>
-  <si>
     <t>Giulia Maia</t>
   </si>
   <si>
@@ -494,6 +468,57 @@
   </si>
   <si>
     <t>Testar os cenários de avisos</t>
+  </si>
+  <si>
+    <t>Email do cliente = fausto@gmail.com</t>
+  </si>
+  <si>
+    <t>Email do usuário =  fausto@gmail.com</t>
+  </si>
+  <si>
+    <t>Email do usuário =  fausto1@gmail.com</t>
+  </si>
+  <si>
+    <t>Entrar no site https://nodepharmasensors.azurewebsites.net</t>
+  </si>
+  <si>
+    <t>Selecionar no menu a opção Login</t>
+  </si>
+  <si>
+    <t>Digitar uma senha válida e clicar no botão Entrar</t>
+  </si>
+  <si>
+    <t>Abrir o site institucional do PharmaSensors, clicar na opção do menu 'login'; inserir o email do usuário no campo e-mail; não inserir o campo senha</t>
+  </si>
+  <si>
+    <t>Exibir a mensagem de erro "Preencha esse campo!"; voltar para campo Login</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mostrar gráficos de medicamentocomum </t>
+  </si>
+  <si>
+    <t>Abrir o site; Logar o usuário teste; inserir no banco temperaturas para teste; Entrar na aba tempo real; Entrar no Comum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Visualizar a temperatura e umidade </t>
+  </si>
+  <si>
+    <t>Abrir o site; Logar o usuário teste; inserir no banco temperaturas para teste; Entrar na aba tempo real; Entrar no insulinas</t>
+  </si>
+  <si>
+    <t>Abrir o site; Logar o usuário teste; inserir no banco temperaturas para teste; Entrar na aba tempo real; Entrar no imunobiológicos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mostrar gráficos de insulinas </t>
+  </si>
+  <si>
+    <t>Mostrar gráficos de imunobiológicos</t>
+  </si>
+  <si>
+    <t>RF-04-06</t>
+  </si>
+  <si>
+    <t>Testar os cenários dos gráficos</t>
   </si>
 </sst>
 </file>
@@ -770,7 +795,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -828,12 +853,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.59999389629810485"/>
-        <bgColor indexed="26"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="26"/>
       </patternFill>
     </fill>
@@ -1365,51 +1384,168 @@
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="12" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="24" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="23" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="9" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="2" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="2" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="37" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="2" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="41" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="12" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="2" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="2" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="2" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="2" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="2" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="30" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1436,55 +1572,6 @@
     <xf numFmtId="0" fontId="15" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="2" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="2" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="2" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="2" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="2" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="2" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1494,32 +1581,6 @@
     <xf numFmtId="0" fontId="17" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="2" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="23" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
@@ -1528,6 +1589,10 @@
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="42" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1554,52 +1619,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="9" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="2" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="15">
@@ -1705,58 +1724,14 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>297763</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>180382</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>1904999</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>979716</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Imagem 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="11414799" y="4942882"/>
-          <a:ext cx="1607236" cy="799334"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>5</xdr:col>
       <xdr:colOff>217713</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>40821</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1973034</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>884464</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1773,7 +1748,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1782,6 +1757,676 @@
         <a:xfrm>
           <a:off x="11538856" y="9375321"/>
           <a:ext cx="1755321" cy="843643"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>204109</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>42375</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1973036</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>908524</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Imagem 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{39B8C669-F5BE-4EDB-8FE2-2D2BE0C81E0D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11525252" y="8424375"/>
+          <a:ext cx="1768927" cy="866149"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>231322</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>54912</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1961758</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>1077440</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Imagem 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A3BFEF7D-02E6-43B0-9F18-1286CAE0DD9E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11552465" y="6150912"/>
+          <a:ext cx="1730436" cy="1022528"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>40822</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>81643</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2145199</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>979714</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Imagem 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{849C8BF8-7169-432A-94D0-68C3436D9AD4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11361965" y="5034643"/>
+          <a:ext cx="2104377" cy="898071"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>489857</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>98938</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1646462</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>1102180</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Imagem 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4B75526B-2D24-4909-9C11-0DAFB25C3AB2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11811000" y="7337938"/>
+          <a:ext cx="1156605" cy="1003242"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>489859</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1592036</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>1041751</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Imagem 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9F52BDA3-6664-4F0B-B178-7460C51A6D83}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11811002" y="7334250"/>
+          <a:ext cx="1102177" cy="946501"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>108197</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>247650</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2105025</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>875850</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagem 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F066F09D-2F9B-4011-83CB-D457C4FB7F6F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6585197" y="6305550"/>
+          <a:ext cx="1996828" cy="628200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>123826</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>42795</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2028825</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>647700</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagem 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D92D3386-F9DC-444C-A4F4-3FBDD0D6054B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6600826" y="4367145"/>
+          <a:ext cx="1904999" cy="604905"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>152764</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>66828</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1981200</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>613672</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Imagem 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BF82EA45-338F-4823-8B71-12BB2292374C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6629764" y="3724428"/>
+          <a:ext cx="1828436" cy="546844"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>47626</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2143125</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>828675</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Imagem 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F6BA4506-A0AF-44FC-88BA-CBC4E908CBEB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6524626" y="5172075"/>
+          <a:ext cx="2095499" cy="647700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>19052</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>15992</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1133475</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>527422</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Imagem 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C2775B64-C01D-4F81-ABEF-79925F93162D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6496052" y="3673592"/>
+          <a:ext cx="1114423" cy="511430"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1133474</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>350311</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2143125</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>783767</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Imagem 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E73FE92A-8532-4AD5-9192-5F10C3305BCC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7610474" y="4007911"/>
+          <a:ext cx="1009651" cy="433456"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1143000</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>219075</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2152651</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>652531</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Imagem 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3BF804B6-80C8-4BB2-90B3-E66A42452A3E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7620000" y="4676775"/>
+          <a:ext cx="1009651" cy="433456"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1133475</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>352425</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2143126</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>785881</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Imagem 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{59EBDE39-3C74-495D-9273-D0F0F0AA133A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7610475" y="5610225"/>
+          <a:ext cx="1009651" cy="433456"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>12611</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>11194</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1143001</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>520244</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Imagem 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8ABA7139-BA0A-4CEF-8F3E-479088EF6744}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6489611" y="4468894"/>
+          <a:ext cx="1130390" cy="509050"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>11718</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>9526</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1152526</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>522596</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Imagem 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{076CD506-265C-4D9B-9C01-24DD13E1C179}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6488718" y="5267326"/>
+          <a:ext cx="1140808" cy="513070"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2154,13 +2799,13 @@
     </row>
     <row r="2" spans="1:20" s="22" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="50"/>
-      <c r="B2" s="85" t="s">
+      <c r="B2" s="117" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="86"/>
-      <c r="D2" s="86"/>
-      <c r="E2" s="86"/>
-      <c r="F2" s="87"/>
+      <c r="C2" s="118"/>
+      <c r="D2" s="118"/>
+      <c r="E2" s="118"/>
+      <c r="F2" s="119"/>
       <c r="G2" s="54"/>
       <c r="H2" s="54"/>
       <c r="I2" s="54"/>
@@ -2170,11 +2815,11 @@
     </row>
     <row r="3" spans="1:20" s="22" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="50"/>
-      <c r="B3" s="88"/>
-      <c r="C3" s="89"/>
-      <c r="D3" s="89"/>
-      <c r="E3" s="89"/>
-      <c r="F3" s="90"/>
+      <c r="B3" s="120"/>
+      <c r="C3" s="121"/>
+      <c r="D3" s="121"/>
+      <c r="E3" s="121"/>
+      <c r="F3" s="122"/>
       <c r="G3" s="54"/>
       <c r="H3" s="54"/>
       <c r="I3" s="54"/>
@@ -2201,10 +2846,10 @@
       <c r="B5" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="91" t="s">
-        <v>94</v>
-      </c>
-      <c r="D5" s="92"/>
+      <c r="C5" s="123" t="s">
+        <v>90</v>
+      </c>
+      <c r="D5" s="124"/>
       <c r="E5" s="27"/>
       <c r="F5" s="28"/>
       <c r="G5" s="27"/>
@@ -2219,8 +2864,8 @@
       <c r="B6" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="91"/>
-      <c r="D6" s="92"/>
+      <c r="C6" s="123"/>
+      <c r="D6" s="124"/>
       <c r="E6" s="27"/>
       <c r="F6" s="28"/>
       <c r="G6" s="27"/>
@@ -2235,8 +2880,8 @@
       <c r="B7" s="58" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="91"/>
-      <c r="D7" s="92"/>
+      <c r="C7" s="123"/>
+      <c r="D7" s="124"/>
       <c r="E7" s="27"/>
       <c r="F7" s="28"/>
       <c r="G7" s="27"/>
@@ -2251,8 +2896,8 @@
       <c r="B8" s="58" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="91"/>
-      <c r="D8" s="92"/>
+      <c r="C8" s="123"/>
+      <c r="D8" s="124"/>
       <c r="E8" s="27"/>
       <c r="F8" s="28"/>
       <c r="G8" s="27"/>
@@ -2265,10 +2910,10 @@
     <row r="9" spans="1:20" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A9" s="23"/>
       <c r="B9" s="58" t="s">
-        <v>92</v>
-      </c>
-      <c r="C9" s="91"/>
-      <c r="D9" s="92"/>
+        <v>88</v>
+      </c>
+      <c r="C9" s="123"/>
+      <c r="D9" s="124"/>
       <c r="E9" s="27"/>
       <c r="F9" s="28"/>
       <c r="G9" s="27"/>
@@ -2294,16 +2939,16 @@
     </row>
     <row r="11" spans="1:20" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="23"/>
-      <c r="B11" s="107" t="s">
-        <v>53</v>
-      </c>
-      <c r="C11" s="108"/>
-      <c r="D11" s="108"/>
-      <c r="E11" s="108"/>
-      <c r="F11" s="108"/>
-      <c r="G11" s="108"/>
-      <c r="H11" s="108"/>
-      <c r="I11" s="109"/>
+      <c r="B11" s="125" t="s">
+        <v>52</v>
+      </c>
+      <c r="C11" s="126"/>
+      <c r="D11" s="126"/>
+      <c r="E11" s="126"/>
+      <c r="F11" s="126"/>
+      <c r="G11" s="126"/>
+      <c r="H11" s="126"/>
+      <c r="I11" s="127"/>
       <c r="J11" s="27"/>
       <c r="K11" s="27"/>
       <c r="L11" s="23"/>
@@ -2313,16 +2958,16 @@
     <row r="12" spans="1:20" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A12" s="51"/>
       <c r="B12" s="69" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" s="108" t="s">
         <v>46</v>
       </c>
-      <c r="C12" s="101" t="s">
+      <c r="D12" s="109"/>
+      <c r="E12" s="108" t="s">
         <v>47</v>
       </c>
-      <c r="D12" s="102"/>
-      <c r="E12" s="101" t="s">
-        <v>48</v>
-      </c>
-      <c r="F12" s="102"/>
+      <c r="F12" s="109"/>
       <c r="G12" s="69" t="s">
         <v>24</v>
       </c>
@@ -2343,21 +2988,21 @@
     <row r="13" spans="1:20" s="4" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="51"/>
       <c r="B13" s="60" t="s">
-        <v>49</v>
-      </c>
-      <c r="C13" s="93" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13" s="98" t="s">
+        <v>56</v>
+      </c>
+      <c r="D13" s="99"/>
+      <c r="E13" s="102" t="s">
         <v>57</v>
       </c>
-      <c r="D13" s="94"/>
-      <c r="E13" s="95" t="s">
-        <v>58</v>
-      </c>
-      <c r="F13" s="103"/>
+      <c r="F13" s="110"/>
       <c r="G13" s="61" t="s">
+        <v>53</v>
+      </c>
+      <c r="H13" s="61" t="s">
         <v>54</v>
-      </c>
-      <c r="H13" s="61" t="s">
-        <v>55</v>
       </c>
       <c r="I13" s="61"/>
       <c r="J13" s="59"/>
@@ -2371,16 +3016,16 @@
     <row r="14" spans="1:20" s="4" customFormat="1" ht="41.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="51"/>
       <c r="B14" s="70" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C14" s="115" t="s">
+        <v>58</v>
+      </c>
+      <c r="D14" s="116"/>
+      <c r="E14" s="111" t="s">
         <v>59</v>
       </c>
-      <c r="D14" s="116"/>
-      <c r="E14" s="104" t="s">
-        <v>60</v>
-      </c>
-      <c r="F14" s="105"/>
+      <c r="F14" s="112"/>
       <c r="G14" s="71"/>
       <c r="H14" s="71"/>
       <c r="I14" s="71"/>
@@ -2395,16 +3040,16 @@
     <row r="15" spans="1:20" s="4" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="51"/>
       <c r="B15" s="60" t="s">
-        <v>51</v>
-      </c>
-      <c r="C15" s="93" t="s">
+        <v>50</v>
+      </c>
+      <c r="C15" s="98" t="s">
+        <v>60</v>
+      </c>
+      <c r="D15" s="99"/>
+      <c r="E15" s="98" t="s">
         <v>61</v>
       </c>
-      <c r="D15" s="94"/>
-      <c r="E15" s="93" t="s">
-        <v>62</v>
-      </c>
-      <c r="F15" s="106"/>
+      <c r="F15" s="101"/>
       <c r="G15" s="61"/>
       <c r="H15" s="61"/>
       <c r="I15" s="61"/>
@@ -2419,12 +3064,12 @@
     <row r="16" spans="1:20" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A16" s="51"/>
       <c r="B16" s="60" t="s">
-        <v>52</v>
-      </c>
-      <c r="C16" s="93"/>
-      <c r="D16" s="94"/>
-      <c r="E16" s="93"/>
-      <c r="F16" s="106"/>
+        <v>51</v>
+      </c>
+      <c r="C16" s="98"/>
+      <c r="D16" s="99"/>
+      <c r="E16" s="98"/>
+      <c r="F16" s="101"/>
       <c r="G16" s="61"/>
       <c r="H16" s="61"/>
       <c r="I16" s="61"/>
@@ -2456,17 +3101,17 @@
     </row>
     <row r="18" spans="1:21" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="52"/>
-      <c r="B18" s="110" t="s">
-        <v>56</v>
-      </c>
-      <c r="C18" s="111"/>
-      <c r="D18" s="111"/>
-      <c r="E18" s="111"/>
-      <c r="F18" s="111"/>
-      <c r="G18" s="111"/>
-      <c r="H18" s="111"/>
-      <c r="I18" s="111"/>
-      <c r="J18" s="111"/>
+      <c r="B18" s="113" t="s">
+        <v>55</v>
+      </c>
+      <c r="C18" s="114"/>
+      <c r="D18" s="114"/>
+      <c r="E18" s="114"/>
+      <c r="F18" s="114"/>
+      <c r="G18" s="114"/>
+      <c r="H18" s="114"/>
+      <c r="I18" s="114"/>
+      <c r="J18" s="114"/>
       <c r="K18" s="23"/>
       <c r="L18" s="23"/>
     </row>
@@ -2475,18 +3120,18 @@
       <c r="B19" s="68" t="s">
         <v>21</v>
       </c>
-      <c r="C19" s="97" t="s">
+      <c r="C19" s="106" t="s">
         <v>20</v>
       </c>
-      <c r="D19" s="98"/>
-      <c r="E19" s="97" t="s">
+      <c r="D19" s="107"/>
+      <c r="E19" s="106" t="s">
         <v>22</v>
       </c>
-      <c r="F19" s="98"/>
-      <c r="G19" s="97" t="s">
+      <c r="F19" s="107"/>
+      <c r="G19" s="106" t="s">
         <v>23</v>
       </c>
-      <c r="H19" s="98"/>
+      <c r="H19" s="107"/>
       <c r="I19" s="68" t="s">
         <v>26</v>
       </c>
@@ -2503,20 +3148,20 @@
     <row r="20" spans="1:21" s="4" customFormat="1" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="51"/>
       <c r="B20" s="60" t="s">
+        <v>62</v>
+      </c>
+      <c r="C20" s="98" t="s">
         <v>63</v>
       </c>
-      <c r="C20" s="93" t="s">
+      <c r="D20" s="99"/>
+      <c r="E20" s="98" t="s">
         <v>64</v>
       </c>
-      <c r="D20" s="94"/>
-      <c r="E20" s="93" t="s">
+      <c r="F20" s="99"/>
+      <c r="G20" s="98" t="s">
         <v>65</v>
       </c>
-      <c r="F20" s="94"/>
-      <c r="G20" s="93" t="s">
-        <v>66</v>
-      </c>
-      <c r="H20" s="94"/>
+      <c r="H20" s="99"/>
       <c r="I20" s="62"/>
       <c r="J20" s="61"/>
       <c r="K20" s="26"/>
@@ -2529,20 +3174,20 @@
     <row r="21" spans="1:21" s="4" customFormat="1" ht="70.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="51"/>
       <c r="B21" s="60" t="s">
+        <v>66</v>
+      </c>
+      <c r="C21" s="98" t="s">
         <v>67</v>
       </c>
-      <c r="C21" s="93" t="s">
+      <c r="D21" s="100"/>
+      <c r="E21" s="102" t="s">
         <v>68</v>
       </c>
-      <c r="D21" s="114"/>
-      <c r="E21" s="95" t="s">
-        <v>69</v>
-      </c>
-      <c r="F21" s="96"/>
-      <c r="G21" s="99" t="s">
-        <v>72</v>
-      </c>
-      <c r="H21" s="100"/>
+      <c r="F21" s="103"/>
+      <c r="G21" s="104" t="s">
+        <v>71</v>
+      </c>
+      <c r="H21" s="105"/>
       <c r="I21" s="63"/>
       <c r="J21" s="61"/>
       <c r="K21" s="26"/>
@@ -2555,20 +3200,20 @@
     <row r="22" spans="1:21" s="4" customFormat="1" ht="77.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="51"/>
       <c r="B22" s="60" t="s">
-        <v>67</v>
-      </c>
-      <c r="C22" s="93" t="s">
+        <v>66</v>
+      </c>
+      <c r="C22" s="98" t="s">
+        <v>69</v>
+      </c>
+      <c r="D22" s="100"/>
+      <c r="E22" s="102" t="s">
         <v>70</v>
       </c>
-      <c r="D22" s="114"/>
-      <c r="E22" s="95" t="s">
-        <v>71</v>
-      </c>
-      <c r="F22" s="96"/>
-      <c r="G22" s="99" t="s">
-        <v>73</v>
-      </c>
-      <c r="H22" s="100"/>
+      <c r="F22" s="103"/>
+      <c r="G22" s="104" t="s">
+        <v>72</v>
+      </c>
+      <c r="H22" s="105"/>
       <c r="I22" s="63"/>
       <c r="J22" s="61"/>
       <c r="K22" s="26"/>
@@ -2581,12 +3226,12 @@
     <row r="23" spans="1:21" s="4" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A23" s="51"/>
       <c r="B23" s="60"/>
-      <c r="C23" s="93"/>
-      <c r="D23" s="94"/>
-      <c r="E23" s="93"/>
-      <c r="F23" s="106"/>
-      <c r="G23" s="112"/>
-      <c r="H23" s="113"/>
+      <c r="C23" s="98"/>
+      <c r="D23" s="99"/>
+      <c r="E23" s="98"/>
+      <c r="F23" s="101"/>
+      <c r="G23" s="96"/>
+      <c r="H23" s="97"/>
       <c r="I23" s="63"/>
       <c r="J23" s="61"/>
       <c r="K23" s="26"/>
@@ -2728,16 +3373,16 @@
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="B11:I11"/>
     <mergeCell ref="G19:H19"/>
     <mergeCell ref="G20:H20"/>
     <mergeCell ref="G21:H21"/>
@@ -2752,16 +3397,16 @@
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="E19:F19"/>
     <mergeCell ref="C12:D12"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="B11:I11"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="E21:F21"/>
   </mergeCells>
   <dataValidations disablePrompts="1" count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I13:I16" xr:uid="{00000000-0002-0000-0000-000000000000}">
@@ -2782,10 +3427,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:T41"/>
+  <dimension ref="A1:T42"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A39" sqref="A1:L39"/>
+    <sheetView topLeftCell="A26" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.7109375" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2813,28 +3458,28 @@
         <v>0</v>
       </c>
       <c r="B1" s="31" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.2">
-      <c r="A2" s="83" t="s">
-        <v>40</v>
+      <c r="A2" s="82" t="s">
+        <v>39</v>
       </c>
       <c r="B2" s="31" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="30" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B3" s="31" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="30" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B4" s="35">
         <v>43598</v>
@@ -2842,10 +3487,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="30" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B5" s="36" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -2858,21 +3503,21 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="37" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B9" s="37" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="36" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B10" s="38"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="36" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B11" s="38"/>
     </row>
@@ -2886,35 +3531,35 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="39" t="s">
-        <v>33</v>
-      </c>
-      <c r="B15" s="117" t="s">
-        <v>105</v>
-      </c>
-      <c r="C15" s="117"/>
+        <v>32</v>
+      </c>
+      <c r="B15" s="128" t="s">
+        <v>98</v>
+      </c>
+      <c r="C15" s="128"/>
       <c r="D15" s="40"/>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A17" s="37" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A18" s="118" t="s">
-        <v>96</v>
-      </c>
-      <c r="B18" s="118"/>
-      <c r="C18" s="118"/>
+      <c r="A18" s="129" t="s">
+        <v>92</v>
+      </c>
+      <c r="B18" s="129"/>
+      <c r="C18" s="129"/>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A19" s="118"/>
-      <c r="B19" s="118"/>
-      <c r="C19" s="118"/>
+      <c r="A19" s="129"/>
+      <c r="B19" s="129"/>
+      <c r="C19" s="129"/>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A20" s="118"/>
-      <c r="B20" s="118"/>
-      <c r="C20" s="118"/>
+      <c r="A20" s="129"/>
+      <c r="B20" s="129"/>
+      <c r="C20" s="129"/>
     </row>
     <row r="24" spans="1:20" s="42" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A24" s="66" t="s">
@@ -2927,13 +3572,13 @@
         <v>4</v>
       </c>
       <c r="D24" s="66" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E24" s="67" t="s">
         <v>3</v>
       </c>
       <c r="F24" s="67" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G24" s="67" t="s">
         <v>8</v>
@@ -2942,7 +3587,7 @@
         <v>7</v>
       </c>
       <c r="I24" s="67" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="Q24" s="43"/>
       <c r="R24" s="43"/>
@@ -2951,29 +3596,29 @@
     </row>
     <row r="25" spans="1:20" s="42" customFormat="1" ht="90" x14ac:dyDescent="0.2">
       <c r="A25" s="41" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B25" s="41" t="s">
-        <v>74</v>
-      </c>
-      <c r="C25" s="82" t="s">
-        <v>97</v>
-      </c>
-      <c r="D25" s="82" t="s">
-        <v>98</v>
-      </c>
-      <c r="E25" s="82" t="s">
-        <v>99</v>
+        <v>73</v>
+      </c>
+      <c r="C25" s="81" t="s">
+        <v>93</v>
+      </c>
+      <c r="D25" s="81" t="s">
+        <v>126</v>
+      </c>
+      <c r="E25" s="81" t="s">
+        <v>94</v>
       </c>
       <c r="F25" s="44"/>
       <c r="G25" s="45" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="H25" s="45" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="I25" s="49" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="Q25" s="43"/>
       <c r="R25" s="43"/>
@@ -2982,27 +3627,29 @@
     </row>
     <row r="26" spans="1:20" s="42" customFormat="1" ht="90" x14ac:dyDescent="0.2">
       <c r="A26" s="41" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B26" s="41" t="s">
-        <v>74</v>
-      </c>
-      <c r="C26" s="82" t="s">
-        <v>97</v>
-      </c>
-      <c r="D26" s="82" t="s">
-        <v>101</v>
-      </c>
-      <c r="E26" s="82" t="s">
-        <v>77</v>
-      </c>
-      <c r="F26" s="73"/>
+        <v>73</v>
+      </c>
+      <c r="C26" s="81" t="s">
+        <v>93</v>
+      </c>
+      <c r="D26" s="81" t="s">
+        <v>127</v>
+      </c>
+      <c r="E26" s="81" t="s">
+        <v>76</v>
+      </c>
+      <c r="F26" s="83"/>
       <c r="G26" s="45" t="s">
-        <v>116</v>
-      </c>
-      <c r="H26" s="45"/>
+        <v>107</v>
+      </c>
+      <c r="H26" s="45" t="s">
+        <v>109</v>
+      </c>
       <c r="I26" s="49" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="Q26" s="43"/>
       <c r="R26" s="43"/>
@@ -3011,56 +3658,60 @@
     </row>
     <row r="27" spans="1:20" s="42" customFormat="1" ht="90" x14ac:dyDescent="0.2">
       <c r="A27" s="41" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="B27" s="41" t="s">
-        <v>74</v>
-      </c>
-      <c r="C27" s="82" t="s">
-        <v>102</v>
-      </c>
-      <c r="D27" s="82" t="s">
-        <v>78</v>
-      </c>
-      <c r="E27" s="82" t="s">
-        <v>103</v>
-      </c>
-      <c r="F27" s="73"/>
+        <v>73</v>
+      </c>
+      <c r="C27" s="81" t="s">
+        <v>131</v>
+      </c>
+      <c r="D27" s="81" t="s">
+        <v>126</v>
+      </c>
+      <c r="E27" s="81" t="s">
+        <v>132</v>
+      </c>
+      <c r="F27" s="83"/>
       <c r="G27" s="45" t="s">
-        <v>116</v>
-      </c>
-      <c r="H27" s="45"/>
+        <v>107</v>
+      </c>
+      <c r="H27" s="45" t="s">
+        <v>109</v>
+      </c>
       <c r="I27" s="49" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="Q27" s="43"/>
       <c r="R27" s="43"/>
       <c r="S27" s="43"/>
       <c r="T27" s="43"/>
     </row>
-    <row r="28" spans="1:20" s="42" customFormat="1" ht="75" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:20" s="42" customFormat="1" ht="90" x14ac:dyDescent="0.2">
       <c r="A28" s="41" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="B28" s="41" t="s">
+        <v>73</v>
+      </c>
+      <c r="C28" s="81" t="s">
+        <v>96</v>
+      </c>
+      <c r="D28" s="81" t="s">
+        <v>77</v>
+      </c>
+      <c r="E28" s="81" t="s">
+        <v>132</v>
+      </c>
+      <c r="F28" s="83"/>
+      <c r="G28" s="45" t="s">
         <v>107</v>
       </c>
-      <c r="C28" s="82" t="s">
-        <v>108</v>
-      </c>
-      <c r="D28" s="82" t="s">
+      <c r="H28" s="45" t="s">
         <v>109</v>
       </c>
-      <c r="E28" s="82" t="s">
-        <v>110</v>
-      </c>
-      <c r="F28" s="73"/>
-      <c r="G28" s="45" t="s">
-        <v>116</v>
-      </c>
-      <c r="H28" s="45"/>
       <c r="I28" s="49" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="Q28" s="43"/>
       <c r="R28" s="43"/>
@@ -3069,124 +3720,156 @@
     </row>
     <row r="29" spans="1:20" s="42" customFormat="1" ht="75" x14ac:dyDescent="0.2">
       <c r="A29" s="41" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="B29" s="41" t="s">
+        <v>100</v>
+      </c>
+      <c r="C29" s="81" t="s">
+        <v>101</v>
+      </c>
+      <c r="D29" s="81" t="s">
+        <v>125</v>
+      </c>
+      <c r="E29" s="81" t="s">
+        <v>102</v>
+      </c>
+      <c r="F29" s="83"/>
+      <c r="G29" s="45" t="s">
         <v>107</v>
       </c>
-      <c r="C29" s="82" t="s">
-        <v>112</v>
-      </c>
-      <c r="D29" s="82" t="s">
+      <c r="H29" s="45" t="s">
         <v>109</v>
       </c>
-      <c r="E29" s="82" t="s">
-        <v>114</v>
-      </c>
-      <c r="F29" s="84"/>
-      <c r="G29" s="45" t="s">
-        <v>31</v>
-      </c>
-      <c r="H29" s="45" t="s">
-        <v>117</v>
-      </c>
       <c r="I29" s="49" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="Q29" s="43"/>
       <c r="R29" s="43"/>
       <c r="S29" s="43"/>
       <c r="T29" s="43"/>
     </row>
-    <row r="30" spans="1:20" s="76" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A30" s="74"/>
-      <c r="B30" s="74"/>
-      <c r="C30" s="75"/>
-      <c r="D30" s="75"/>
-      <c r="E30" s="75"/>
-      <c r="G30" s="77"/>
-      <c r="H30" s="77"/>
-      <c r="I30" s="78"/>
-      <c r="Q30" s="81"/>
-      <c r="R30" s="81"/>
-      <c r="S30" s="81"/>
-      <c r="T30" s="81"/>
-    </row>
-    <row r="31" spans="1:20" s="42" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A31" s="74"/>
-      <c r="B31" s="74"/>
-      <c r="C31" s="75"/>
-      <c r="D31" s="75"/>
-      <c r="E31" s="75"/>
-      <c r="F31" s="76"/>
-      <c r="G31" s="77"/>
-      <c r="H31" s="77"/>
-      <c r="I31" s="78"/>
-      <c r="Q31" s="43"/>
-      <c r="R31" s="43"/>
-      <c r="S31" s="43"/>
-      <c r="T31" s="43"/>
-    </row>
-    <row r="32" spans="1:20" s="42" customFormat="1" ht="70.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="74"/>
-      <c r="B32" s="74"/>
-      <c r="C32" s="75"/>
-      <c r="D32" s="75"/>
-      <c r="E32" s="75"/>
-      <c r="F32" s="76"/>
-      <c r="G32" s="77"/>
-      <c r="H32" s="77"/>
-      <c r="I32" s="78"/>
+    <row r="30" spans="1:20" s="42" customFormat="1" ht="75" x14ac:dyDescent="0.2">
+      <c r="A30" s="41" t="s">
+        <v>140</v>
+      </c>
+      <c r="B30" s="41" t="s">
+        <v>100</v>
+      </c>
+      <c r="C30" s="81" t="s">
+        <v>104</v>
+      </c>
+      <c r="D30" s="81" t="s">
+        <v>125</v>
+      </c>
+      <c r="E30" s="81" t="s">
+        <v>106</v>
+      </c>
+      <c r="F30" s="83"/>
+      <c r="G30" s="45" t="s">
+        <v>107</v>
+      </c>
+      <c r="H30" s="45" t="s">
+        <v>109</v>
+      </c>
+      <c r="I30" s="49" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q30" s="43"/>
+      <c r="R30" s="43"/>
+      <c r="S30" s="43"/>
+      <c r="T30" s="43"/>
+    </row>
+    <row r="31" spans="1:20" s="75" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A31" s="73"/>
+      <c r="B31" s="73"/>
+      <c r="C31" s="74"/>
+      <c r="D31" s="74"/>
+      <c r="E31" s="74"/>
+      <c r="G31" s="76"/>
+      <c r="H31" s="76"/>
+      <c r="I31" s="77"/>
+      <c r="Q31" s="80"/>
+      <c r="R31" s="80"/>
+      <c r="S31" s="80"/>
+      <c r="T31" s="80"/>
+    </row>
+    <row r="32" spans="1:20" s="42" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A32" s="73"/>
+      <c r="B32" s="73"/>
+      <c r="C32" s="74"/>
+      <c r="D32" s="74"/>
+      <c r="E32" s="74"/>
+      <c r="F32" s="75"/>
+      <c r="G32" s="76"/>
+      <c r="H32" s="76"/>
+      <c r="I32" s="77"/>
       <c r="Q32" s="43"/>
       <c r="R32" s="43"/>
       <c r="S32" s="43"/>
       <c r="T32" s="43"/>
     </row>
-    <row r="33" spans="1:20" s="42" customFormat="1" ht="75.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="74"/>
-      <c r="B33" s="74"/>
-      <c r="C33" s="75"/>
-      <c r="D33" s="75"/>
-      <c r="E33" s="75"/>
-      <c r="F33" s="79"/>
-      <c r="G33" s="77"/>
-      <c r="H33" s="77"/>
-      <c r="I33" s="80"/>
+    <row r="33" spans="1:20" s="42" customFormat="1" ht="70.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="73"/>
+      <c r="B33" s="73"/>
+      <c r="C33" s="74"/>
+      <c r="D33" s="74"/>
+      <c r="E33" s="74"/>
+      <c r="F33" s="75"/>
+      <c r="G33" s="76"/>
+      <c r="H33" s="76"/>
+      <c r="I33" s="77"/>
       <c r="Q33" s="43"/>
       <c r="R33" s="43"/>
       <c r="S33" s="43"/>
       <c r="T33" s="43"/>
     </row>
-    <row r="34" spans="1:20" s="42" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:20" s="42" customFormat="1" ht="75.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="73"/>
+      <c r="B34" s="73"/>
+      <c r="C34" s="74"/>
+      <c r="D34" s="74"/>
+      <c r="E34" s="74"/>
+      <c r="F34" s="78"/>
+      <c r="G34" s="76"/>
+      <c r="H34" s="76"/>
+      <c r="I34" s="79"/>
       <c r="Q34" s="43"/>
       <c r="R34" s="43"/>
       <c r="S34" s="43"/>
       <c r="T34" s="43"/>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A36" s="46" t="s">
+    <row r="35" spans="1:20" s="42" customFormat="1" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="Q35" s="43"/>
+      <c r="R35" s="43"/>
+      <c r="S35" s="43"/>
+      <c r="T35" s="43"/>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A37" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="B36" s="32" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A37" s="47" t="s">
+      <c r="B37" s="32" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A38" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="B37" s="48">
-        <v>43612</v>
-      </c>
-    </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A41" s="37"/>
+      <c r="B38" s="48">
+        <v>43618</v>
+      </c>
+    </row>
+    <row r="42" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A42" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="A18:C20"/>
   </mergeCells>
+  <phoneticPr fontId="4" type="noConversion"/>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="0.78749999999999998" bottom="0.78749999999999998" header="0" footer="9.8611111111111122E-2"/>
   <pageSetup fitToHeight="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -3201,8 +3884,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DBF58C3-8032-41F8-900E-C34CBDD67EBE}">
   <dimension ref="A1:L39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3223,7 +3906,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="31" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C1" s="32"/>
       <c r="D1" s="32"/>
@@ -3236,9 +3919,9 @@
       <c r="K1" s="32"/>
       <c r="L1" s="32"/>
     </row>
-    <row r="2" spans="1:12" ht="60" x14ac:dyDescent="0.2">
-      <c r="A2" s="83" t="s">
-        <v>40</v>
+    <row r="2" spans="1:12" ht="30" x14ac:dyDescent="0.2">
+      <c r="A2" s="82" t="s">
+        <v>39</v>
       </c>
       <c r="B2" s="31"/>
       <c r="C2" s="32"/>
@@ -3254,10 +3937,10 @@
     </row>
     <row r="3" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="30" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B3" s="31" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="C3" s="32"/>
       <c r="D3" s="32"/>
@@ -3272,7 +3955,7 @@
     </row>
     <row r="4" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="30" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B4" s="35">
         <v>43615</v>
@@ -3290,10 +3973,10 @@
     </row>
     <row r="5" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="30" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B5" s="36" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C5" s="32"/>
       <c r="D5" s="32"/>
@@ -3434,12 +4117,12 @@
     </row>
     <row r="15" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" s="39" t="s">
-        <v>33</v>
-      </c>
-      <c r="B15" s="139" t="s">
-        <v>133</v>
-      </c>
-      <c r="C15" s="139"/>
+        <v>32</v>
+      </c>
+      <c r="B15" s="130" t="s">
+        <v>124</v>
+      </c>
+      <c r="C15" s="130"/>
       <c r="D15" s="72"/>
       <c r="E15" s="32"/>
       <c r="F15" s="33"/>
@@ -3466,7 +4149,7 @@
     </row>
     <row r="17" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A17" s="37" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B17" s="32"/>
       <c r="C17" s="32"/>
@@ -3481,11 +4164,11 @@
       <c r="L17" s="32"/>
     </row>
     <row r="18" spans="1:12" ht="15" x14ac:dyDescent="0.2">
-      <c r="A18" s="118" t="s">
-        <v>96</v>
-      </c>
-      <c r="B18" s="118"/>
-      <c r="C18" s="118"/>
+      <c r="A18" s="129" t="s">
+        <v>92</v>
+      </c>
+      <c r="B18" s="129"/>
+      <c r="C18" s="129"/>
       <c r="D18" s="32"/>
       <c r="E18" s="32"/>
       <c r="F18" s="33"/>
@@ -3497,9 +4180,9 @@
       <c r="L18" s="32"/>
     </row>
     <row r="19" spans="1:12" ht="15" x14ac:dyDescent="0.2">
-      <c r="A19" s="118"/>
-      <c r="B19" s="118"/>
-      <c r="C19" s="118"/>
+      <c r="A19" s="129"/>
+      <c r="B19" s="129"/>
+      <c r="C19" s="129"/>
       <c r="D19" s="32"/>
       <c r="E19" s="32"/>
       <c r="F19" s="33"/>
@@ -3511,9 +4194,9 @@
       <c r="L19" s="32"/>
     </row>
     <row r="20" spans="1:12" ht="15" x14ac:dyDescent="0.2">
-      <c r="A20" s="118"/>
-      <c r="B20" s="118"/>
-      <c r="C20" s="118"/>
+      <c r="A20" s="129"/>
+      <c r="B20" s="129"/>
+      <c r="C20" s="129"/>
       <c r="D20" s="32"/>
       <c r="E20" s="32"/>
       <c r="F20" s="33"/>
@@ -3566,216 +4249,224 @@
       <c r="K23" s="32"/>
       <c r="L23" s="32"/>
     </row>
-    <row r="24" spans="1:12" s="25" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="A24" s="128" t="s">
+    <row r="24" spans="1:12" s="25" customFormat="1" ht="33.75" x14ac:dyDescent="0.2">
+      <c r="A24" s="85" t="s">
         <v>1</v>
       </c>
-      <c r="B24" s="128" t="s">
+      <c r="B24" s="85" t="s">
         <v>2</v>
       </c>
-      <c r="C24" s="128" t="s">
+      <c r="C24" s="85" t="s">
         <v>4</v>
       </c>
-      <c r="D24" s="128" t="s">
-        <v>43</v>
-      </c>
-      <c r="E24" s="129" t="s">
+      <c r="D24" s="85" t="s">
+        <v>42</v>
+      </c>
+      <c r="E24" s="86" t="s">
         <v>3</v>
       </c>
-      <c r="F24" s="129" t="s">
+      <c r="F24" s="86" t="s">
+        <v>40</v>
+      </c>
+      <c r="G24" s="86" t="s">
+        <v>8</v>
+      </c>
+      <c r="H24" s="86" t="s">
+        <v>7</v>
+      </c>
+      <c r="I24" s="86" t="s">
         <v>41</v>
-      </c>
-      <c r="G24" s="129" t="s">
-        <v>8</v>
-      </c>
-      <c r="H24" s="129" t="s">
-        <v>7</v>
-      </c>
-      <c r="I24" s="129" t="s">
-        <v>42</v>
       </c>
       <c r="J24" s="26"/>
       <c r="K24" s="26"/>
       <c r="L24" s="26"/>
     </row>
-    <row r="25" spans="1:12" s="135" customFormat="1" ht="52.5" x14ac:dyDescent="0.2">
-      <c r="A25" s="130" t="s">
+    <row r="25" spans="1:12" s="92" customFormat="1" ht="52.5" x14ac:dyDescent="0.2">
+      <c r="A25" s="87" t="s">
+        <v>112</v>
+      </c>
+      <c r="B25" s="87" t="s">
+        <v>116</v>
+      </c>
+      <c r="C25" s="88" t="s">
+        <v>120</v>
+      </c>
+      <c r="D25" s="88" t="s">
         <v>121</v>
       </c>
-      <c r="B25" s="130" t="s">
-        <v>125</v>
-      </c>
-      <c r="C25" s="131" t="s">
-        <v>129</v>
-      </c>
-      <c r="D25" s="131" t="s">
-        <v>130</v>
-      </c>
-      <c r="E25" s="131" t="s">
-        <v>131</v>
-      </c>
-      <c r="F25" s="132"/>
-      <c r="G25" s="133" t="s">
-        <v>116</v>
-      </c>
-      <c r="H25" s="133"/>
-      <c r="I25" s="134" t="s">
-        <v>44</v>
+      <c r="E25" s="88" t="s">
+        <v>122</v>
+      </c>
+      <c r="F25" s="89"/>
+      <c r="G25" s="90" t="s">
+        <v>108</v>
+      </c>
+      <c r="H25" s="90" t="s">
+        <v>109</v>
+      </c>
+      <c r="I25" s="91" t="s">
+        <v>43</v>
       </c>
       <c r="J25" s="4"/>
       <c r="K25" s="4"/>
       <c r="L25" s="4"/>
     </row>
-    <row r="26" spans="1:12" s="135" customFormat="1" ht="52.5" x14ac:dyDescent="0.2">
-      <c r="A26" s="130" t="s">
+    <row r="26" spans="1:12" s="92" customFormat="1" ht="52.5" x14ac:dyDescent="0.2">
+      <c r="A26" s="87" t="s">
+        <v>113</v>
+      </c>
+      <c r="B26" s="87" t="s">
+        <v>117</v>
+      </c>
+      <c r="C26" s="88" t="s">
+        <v>120</v>
+      </c>
+      <c r="D26" s="88" t="s">
+        <v>121</v>
+      </c>
+      <c r="E26" s="88" t="s">
         <v>122</v>
       </c>
-      <c r="B26" s="130" t="s">
-        <v>126</v>
-      </c>
-      <c r="C26" s="131" t="s">
-        <v>129</v>
-      </c>
-      <c r="D26" s="131" t="s">
-        <v>130</v>
-      </c>
-      <c r="E26" s="131" t="s">
-        <v>131</v>
-      </c>
-      <c r="F26" s="136"/>
-      <c r="G26" s="133" t="s">
-        <v>116</v>
-      </c>
-      <c r="H26" s="133"/>
-      <c r="I26" s="134" t="s">
-        <v>44</v>
+      <c r="F26" s="93"/>
+      <c r="G26" s="90" t="s">
+        <v>108</v>
+      </c>
+      <c r="H26" s="90" t="s">
+        <v>109</v>
+      </c>
+      <c r="I26" s="91" t="s">
+        <v>43</v>
       </c>
       <c r="J26" s="4"/>
       <c r="K26" s="4"/>
       <c r="L26" s="4"/>
     </row>
-    <row r="27" spans="1:12" s="135" customFormat="1" ht="84" x14ac:dyDescent="0.2">
-      <c r="A27" s="130" t="s">
+    <row r="27" spans="1:12" s="92" customFormat="1" ht="84" x14ac:dyDescent="0.2">
+      <c r="A27" s="87" t="s">
+        <v>114</v>
+      </c>
+      <c r="B27" s="87" t="s">
+        <v>119</v>
+      </c>
+      <c r="C27" s="88" t="s">
+        <v>120</v>
+      </c>
+      <c r="D27" s="88" t="s">
+        <v>121</v>
+      </c>
+      <c r="E27" s="88" t="s">
         <v>123</v>
       </c>
-      <c r="B27" s="130" t="s">
-        <v>128</v>
-      </c>
-      <c r="C27" s="131" t="s">
-        <v>129</v>
-      </c>
-      <c r="D27" s="131" t="s">
-        <v>130</v>
-      </c>
-      <c r="E27" s="131" t="s">
-        <v>132</v>
-      </c>
-      <c r="F27" s="136"/>
-      <c r="G27" s="133" t="s">
-        <v>116</v>
-      </c>
-      <c r="H27" s="133"/>
-      <c r="I27" s="134" t="s">
-        <v>44</v>
+      <c r="F27" s="93"/>
+      <c r="G27" s="90" t="s">
+        <v>108</v>
+      </c>
+      <c r="H27" s="90" t="s">
+        <v>109</v>
+      </c>
+      <c r="I27" s="91" t="s">
+        <v>43</v>
       </c>
       <c r="J27" s="4"/>
       <c r="K27" s="4"/>
       <c r="L27" s="4"/>
     </row>
-    <row r="28" spans="1:12" s="135" customFormat="1" ht="84" x14ac:dyDescent="0.2">
-      <c r="A28" s="130" t="s">
-        <v>124</v>
-      </c>
-      <c r="B28" s="130" t="s">
-        <v>127</v>
-      </c>
-      <c r="C28" s="131" t="s">
-        <v>129</v>
-      </c>
-      <c r="D28" s="131" t="s">
-        <v>130</v>
-      </c>
-      <c r="E28" s="131" t="s">
-        <v>132</v>
-      </c>
-      <c r="F28" s="136"/>
-      <c r="G28" s="133" t="s">
-        <v>116</v>
-      </c>
-      <c r="H28" s="133"/>
-      <c r="I28" s="134" t="s">
-        <v>44</v>
+    <row r="28" spans="1:12" s="92" customFormat="1" ht="84" x14ac:dyDescent="0.2">
+      <c r="A28" s="87" t="s">
+        <v>115</v>
+      </c>
+      <c r="B28" s="87" t="s">
+        <v>118</v>
+      </c>
+      <c r="C28" s="88" t="s">
+        <v>120</v>
+      </c>
+      <c r="D28" s="88" t="s">
+        <v>121</v>
+      </c>
+      <c r="E28" s="88" t="s">
+        <v>123</v>
+      </c>
+      <c r="F28" s="93"/>
+      <c r="G28" s="90" t="s">
+        <v>108</v>
+      </c>
+      <c r="H28" s="90" t="s">
+        <v>109</v>
+      </c>
+      <c r="I28" s="91" t="s">
+        <v>43</v>
       </c>
       <c r="J28" s="4"/>
       <c r="K28" s="4"/>
       <c r="L28" s="4"/>
     </row>
-    <row r="29" spans="1:12" s="135" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="A29" s="130"/>
-      <c r="B29" s="130"/>
-      <c r="C29" s="131"/>
-      <c r="D29" s="131"/>
-      <c r="E29" s="131"/>
-      <c r="F29" s="136"/>
-      <c r="G29" s="133"/>
-      <c r="H29" s="133"/>
-      <c r="I29" s="134"/>
+    <row r="29" spans="1:12" s="92" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="A29" s="87"/>
+      <c r="B29" s="87"/>
+      <c r="C29" s="88"/>
+      <c r="D29" s="88"/>
+      <c r="E29" s="88"/>
+      <c r="F29" s="93"/>
+      <c r="G29" s="90"/>
+      <c r="H29" s="90"/>
+      <c r="I29" s="91"/>
       <c r="J29" s="4"/>
       <c r="K29" s="4"/>
       <c r="L29" s="4"/>
     </row>
     <row r="30" spans="1:12" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A30" s="74"/>
-      <c r="B30" s="74"/>
-      <c r="C30" s="75"/>
-      <c r="D30" s="75"/>
-      <c r="E30" s="75"/>
-      <c r="F30" s="76"/>
-      <c r="G30" s="77"/>
-      <c r="H30" s="77"/>
-      <c r="I30" s="78"/>
-      <c r="J30" s="76"/>
-      <c r="K30" s="76"/>
-      <c r="L30" s="76"/>
+      <c r="A30" s="73"/>
+      <c r="B30" s="73"/>
+      <c r="C30" s="74"/>
+      <c r="D30" s="74"/>
+      <c r="E30" s="74"/>
+      <c r="F30" s="75"/>
+      <c r="G30" s="76"/>
+      <c r="H30" s="76"/>
+      <c r="I30" s="77"/>
+      <c r="J30" s="75"/>
+      <c r="K30" s="75"/>
+      <c r="L30" s="75"/>
     </row>
     <row r="31" spans="1:12" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A31" s="74"/>
-      <c r="B31" s="74"/>
-      <c r="C31" s="75"/>
-      <c r="D31" s="75"/>
-      <c r="E31" s="75"/>
-      <c r="F31" s="76"/>
-      <c r="G31" s="77"/>
-      <c r="H31" s="77"/>
-      <c r="I31" s="78"/>
+      <c r="A31" s="73"/>
+      <c r="B31" s="73"/>
+      <c r="C31" s="74"/>
+      <c r="D31" s="74"/>
+      <c r="E31" s="74"/>
+      <c r="F31" s="75"/>
+      <c r="G31" s="76"/>
+      <c r="H31" s="76"/>
+      <c r="I31" s="77"/>
       <c r="J31" s="42"/>
       <c r="K31" s="42"/>
       <c r="L31" s="42"/>
     </row>
     <row r="32" spans="1:12" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A32" s="74"/>
-      <c r="B32" s="74"/>
-      <c r="C32" s="75"/>
-      <c r="D32" s="75"/>
-      <c r="E32" s="75"/>
-      <c r="F32" s="76"/>
-      <c r="G32" s="77"/>
-      <c r="H32" s="77"/>
-      <c r="I32" s="78"/>
+      <c r="A32" s="73"/>
+      <c r="B32" s="73"/>
+      <c r="C32" s="74"/>
+      <c r="D32" s="74"/>
+      <c r="E32" s="74"/>
+      <c r="F32" s="75"/>
+      <c r="G32" s="76"/>
+      <c r="H32" s="76"/>
+      <c r="I32" s="77"/>
       <c r="J32" s="42"/>
       <c r="K32" s="42"/>
       <c r="L32" s="42"/>
     </row>
     <row r="33" spans="1:12" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A33" s="74"/>
-      <c r="B33" s="74"/>
-      <c r="C33" s="75"/>
-      <c r="D33" s="75"/>
-      <c r="E33" s="75"/>
-      <c r="F33" s="79"/>
-      <c r="G33" s="77"/>
-      <c r="H33" s="77"/>
-      <c r="I33" s="80"/>
+      <c r="A33" s="73"/>
+      <c r="B33" s="73"/>
+      <c r="C33" s="74"/>
+      <c r="D33" s="74"/>
+      <c r="E33" s="74"/>
+      <c r="F33" s="78"/>
+      <c r="G33" s="76"/>
+      <c r="H33" s="76"/>
+      <c r="I33" s="79"/>
       <c r="J33" s="42"/>
       <c r="K33" s="42"/>
       <c r="L33" s="42"/>
@@ -3809,11 +4500,11 @@
       <c r="L35" s="32"/>
     </row>
     <row r="36" spans="1:12" ht="15" x14ac:dyDescent="0.2">
-      <c r="A36" s="137" t="s">
+      <c r="A36" s="94" t="s">
         <v>5</v>
       </c>
       <c r="B36" s="32" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="C36" s="32"/>
       <c r="D36" s="32"/>
@@ -3827,7 +4518,7 @@
       <c r="L36" s="32"/>
     </row>
     <row r="37" spans="1:12" ht="15" x14ac:dyDescent="0.2">
-      <c r="A37" s="138" t="s">
+      <c r="A37" s="95" t="s">
         <v>6</v>
       </c>
       <c r="B37" s="48">
@@ -3879,15 +4570,693 @@
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAB3FC0C-3FBA-4C85-92B5-D4EFACF612C5}">
+  <dimension ref="A1:L39"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="23.85546875" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.28515625" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" customWidth="1"/>
+    <col min="5" max="5" width="21.85546875" customWidth="1"/>
+    <col min="6" max="6" width="32.42578125" customWidth="1"/>
+    <col min="7" max="7" width="14" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" customWidth="1"/>
+    <col min="9" max="9" width="17.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="15" x14ac:dyDescent="0.2">
+      <c r="A1" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="31" t="s">
+        <v>90</v>
+      </c>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
+      <c r="K1" s="32"/>
+      <c r="L1" s="32"/>
+    </row>
+    <row r="2" spans="1:12" ht="30" x14ac:dyDescent="0.2">
+      <c r="A2" s="82" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="31"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
+      <c r="L2" s="32"/>
+    </row>
+    <row r="3" spans="1:12" ht="15" x14ac:dyDescent="0.2">
+      <c r="A3" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="31" t="s">
+        <v>110</v>
+      </c>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
+      <c r="K3" s="32"/>
+      <c r="L3" s="32"/>
+    </row>
+    <row r="4" spans="1:12" ht="15" x14ac:dyDescent="0.2">
+      <c r="A4" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="35">
+        <v>43618</v>
+      </c>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="32"/>
+      <c r="I4" s="32"/>
+      <c r="J4" s="32"/>
+      <c r="K4" s="32"/>
+      <c r="L4" s="32"/>
+    </row>
+    <row r="5" spans="1:12" ht="15" x14ac:dyDescent="0.2">
+      <c r="A5" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="32"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="32"/>
+      <c r="H5" s="32"/>
+      <c r="I5" s="32"/>
+      <c r="J5" s="32"/>
+      <c r="K5" s="32"/>
+      <c r="L5" s="32"/>
+    </row>
+    <row r="6" spans="1:12" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="30"/>
+      <c r="B6" s="36"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="33"/>
+      <c r="G6" s="32"/>
+      <c r="H6" s="32"/>
+      <c r="I6" s="32"/>
+      <c r="J6" s="32"/>
+      <c r="K6" s="32"/>
+      <c r="L6" s="32"/>
+    </row>
+    <row r="7" spans="1:12" ht="15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="30"/>
+      <c r="B7" s="36"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="32"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="33"/>
+      <c r="G7" s="32"/>
+      <c r="H7" s="32"/>
+      <c r="I7" s="32"/>
+      <c r="J7" s="32"/>
+      <c r="K7" s="32"/>
+      <c r="L7" s="32"/>
+    </row>
+    <row r="8" spans="1:12" ht="1.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="32"/>
+      <c r="B8" s="32"/>
+      <c r="C8" s="32"/>
+      <c r="D8" s="32"/>
+      <c r="E8" s="32"/>
+      <c r="F8" s="33"/>
+      <c r="G8" s="32"/>
+      <c r="H8" s="32"/>
+      <c r="I8" s="32"/>
+      <c r="J8" s="32"/>
+      <c r="K8" s="32"/>
+      <c r="L8" s="32"/>
+    </row>
+    <row r="9" spans="1:12" ht="15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="37"/>
+      <c r="B9" s="37"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="33"/>
+      <c r="G9" s="32"/>
+      <c r="H9" s="32"/>
+      <c r="I9" s="32"/>
+      <c r="J9" s="32"/>
+      <c r="K9" s="32"/>
+      <c r="L9" s="32"/>
+    </row>
+    <row r="10" spans="1:12" ht="15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="36"/>
+      <c r="B10" s="38"/>
+      <c r="C10" s="32"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="33"/>
+      <c r="G10" s="32"/>
+      <c r="H10" s="32"/>
+      <c r="I10" s="32"/>
+      <c r="J10" s="32"/>
+      <c r="K10" s="32"/>
+      <c r="L10" s="32"/>
+    </row>
+    <row r="11" spans="1:12" ht="15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="36"/>
+      <c r="B11" s="38"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="32"/>
+      <c r="H11" s="32"/>
+      <c r="I11" s="32"/>
+      <c r="J11" s="32"/>
+      <c r="K11" s="32"/>
+      <c r="L11" s="32"/>
+    </row>
+    <row r="12" spans="1:12" ht="15" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="36"/>
+      <c r="B12" s="38"/>
+      <c r="C12" s="32"/>
+      <c r="D12" s="32"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="33"/>
+      <c r="G12" s="32"/>
+      <c r="H12" s="32"/>
+      <c r="I12" s="32"/>
+      <c r="J12" s="32"/>
+      <c r="K12" s="32"/>
+      <c r="L12" s="32"/>
+    </row>
+    <row r="13" spans="1:12" ht="3.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="36"/>
+      <c r="B13" s="38"/>
+      <c r="C13" s="32"/>
+      <c r="D13" s="32"/>
+      <c r="E13" s="32"/>
+      <c r="F13" s="33"/>
+      <c r="G13" s="32"/>
+      <c r="H13" s="32"/>
+      <c r="I13" s="32"/>
+      <c r="J13" s="32"/>
+      <c r="K13" s="32"/>
+      <c r="L13" s="32"/>
+    </row>
+    <row r="14" spans="1:12" ht="15" x14ac:dyDescent="0.2">
+      <c r="A14" s="32"/>
+      <c r="B14" s="32"/>
+      <c r="C14" s="32"/>
+      <c r="D14" s="32"/>
+      <c r="E14" s="32"/>
+      <c r="F14" s="33"/>
+      <c r="G14" s="32"/>
+      <c r="H14" s="32"/>
+      <c r="I14" s="32"/>
+      <c r="J14" s="32"/>
+      <c r="K14" s="32"/>
+      <c r="L14" s="32"/>
+    </row>
+    <row r="15" spans="1:12" ht="15" x14ac:dyDescent="0.2">
+      <c r="A15" s="39" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="130" t="s">
+        <v>141</v>
+      </c>
+      <c r="C15" s="130"/>
+      <c r="D15" s="84"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="33"/>
+      <c r="G15" s="32"/>
+      <c r="H15" s="32"/>
+      <c r="I15" s="32"/>
+      <c r="J15" s="32"/>
+      <c r="K15" s="32"/>
+      <c r="L15" s="32"/>
+    </row>
+    <row r="16" spans="1:12" ht="15" x14ac:dyDescent="0.2">
+      <c r="A16" s="32"/>
+      <c r="B16" s="32"/>
+      <c r="C16" s="32"/>
+      <c r="D16" s="32"/>
+      <c r="E16" s="32"/>
+      <c r="F16" s="33"/>
+      <c r="G16" s="32"/>
+      <c r="H16" s="32"/>
+      <c r="I16" s="32"/>
+      <c r="J16" s="32"/>
+      <c r="K16" s="32"/>
+      <c r="L16" s="32"/>
+    </row>
+    <row r="17" spans="1:12" ht="15" x14ac:dyDescent="0.2">
+      <c r="A17" s="37" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="32"/>
+      <c r="C17" s="32"/>
+      <c r="D17" s="32"/>
+      <c r="E17" s="32"/>
+      <c r="F17" s="33"/>
+      <c r="G17" s="32"/>
+      <c r="H17" s="32"/>
+      <c r="I17" s="32"/>
+      <c r="J17" s="32"/>
+      <c r="K17" s="32"/>
+      <c r="L17" s="32"/>
+    </row>
+    <row r="18" spans="1:12" ht="15" x14ac:dyDescent="0.2">
+      <c r="A18" s="129" t="s">
+        <v>92</v>
+      </c>
+      <c r="B18" s="129"/>
+      <c r="C18" s="129"/>
+      <c r="D18" s="32"/>
+      <c r="E18" s="32"/>
+      <c r="F18" s="33"/>
+      <c r="G18" s="32"/>
+      <c r="H18" s="32"/>
+      <c r="I18" s="32"/>
+      <c r="J18" s="32"/>
+      <c r="K18" s="32"/>
+      <c r="L18" s="32"/>
+    </row>
+    <row r="19" spans="1:12" ht="15" x14ac:dyDescent="0.2">
+      <c r="A19" s="129"/>
+      <c r="B19" s="129"/>
+      <c r="C19" s="129"/>
+      <c r="D19" s="32"/>
+      <c r="E19" s="32"/>
+      <c r="F19" s="33"/>
+      <c r="G19" s="32"/>
+      <c r="H19" s="32"/>
+      <c r="I19" s="32"/>
+      <c r="J19" s="32"/>
+      <c r="K19" s="32"/>
+      <c r="L19" s="32"/>
+    </row>
+    <row r="20" spans="1:12" ht="15" x14ac:dyDescent="0.2">
+      <c r="A20" s="129"/>
+      <c r="B20" s="129"/>
+      <c r="C20" s="129"/>
+      <c r="D20" s="32"/>
+      <c r="E20" s="32"/>
+      <c r="F20" s="33"/>
+      <c r="G20" s="32"/>
+      <c r="H20" s="32"/>
+      <c r="I20" s="32"/>
+      <c r="J20" s="32"/>
+      <c r="K20" s="32"/>
+      <c r="L20" s="32"/>
+    </row>
+    <row r="21" spans="1:12" ht="15" x14ac:dyDescent="0.2">
+      <c r="A21" s="32"/>
+      <c r="B21" s="32"/>
+      <c r="C21" s="32"/>
+      <c r="D21" s="32"/>
+      <c r="E21" s="32"/>
+      <c r="F21" s="33"/>
+      <c r="G21" s="32"/>
+      <c r="H21" s="32"/>
+      <c r="I21" s="32"/>
+      <c r="J21" s="32"/>
+      <c r="K21" s="32"/>
+      <c r="L21" s="32"/>
+    </row>
+    <row r="22" spans="1:12" ht="15" x14ac:dyDescent="0.2">
+      <c r="A22" s="32"/>
+      <c r="B22" s="32"/>
+      <c r="C22" s="32"/>
+      <c r="D22" s="32"/>
+      <c r="E22" s="32"/>
+      <c r="F22" s="33"/>
+      <c r="G22" s="32"/>
+      <c r="H22" s="32"/>
+      <c r="I22" s="32"/>
+      <c r="J22" s="32"/>
+      <c r="K22" s="32"/>
+      <c r="L22" s="32"/>
+    </row>
+    <row r="23" spans="1:12" ht="15" x14ac:dyDescent="0.2">
+      <c r="A23" s="32"/>
+      <c r="B23" s="32"/>
+      <c r="C23" s="32"/>
+      <c r="D23" s="32"/>
+      <c r="E23" s="32"/>
+      <c r="F23" s="33"/>
+      <c r="G23" s="32"/>
+      <c r="H23" s="32"/>
+      <c r="I23" s="32"/>
+      <c r="J23" s="32"/>
+      <c r="K23" s="32"/>
+      <c r="L23" s="32"/>
+    </row>
+    <row r="24" spans="1:12" s="25" customFormat="1" ht="33.75" x14ac:dyDescent="0.2">
+      <c r="A24" s="85" t="s">
+        <v>1</v>
+      </c>
+      <c r="B24" s="85" t="s">
+        <v>2</v>
+      </c>
+      <c r="C24" s="85" t="s">
+        <v>4</v>
+      </c>
+      <c r="D24" s="85" t="s">
+        <v>42</v>
+      </c>
+      <c r="E24" s="86" t="s">
+        <v>3</v>
+      </c>
+      <c r="F24" s="86" t="s">
+        <v>40</v>
+      </c>
+      <c r="G24" s="86" t="s">
+        <v>8</v>
+      </c>
+      <c r="H24" s="86" t="s">
+        <v>7</v>
+      </c>
+      <c r="I24" s="86" t="s">
+        <v>41</v>
+      </c>
+      <c r="J24" s="26"/>
+      <c r="K24" s="26"/>
+      <c r="L24" s="26"/>
+    </row>
+    <row r="25" spans="1:12" s="92" customFormat="1" ht="63" x14ac:dyDescent="0.2">
+      <c r="A25" s="87" t="s">
+        <v>112</v>
+      </c>
+      <c r="B25" s="87" t="s">
+        <v>133</v>
+      </c>
+      <c r="C25" s="88" t="s">
+        <v>134</v>
+      </c>
+      <c r="D25" s="88" t="s">
+        <v>121</v>
+      </c>
+      <c r="E25" s="88" t="s">
+        <v>135</v>
+      </c>
+      <c r="F25" s="89"/>
+      <c r="G25" s="90" t="s">
+        <v>107</v>
+      </c>
+      <c r="H25" s="90" t="s">
+        <v>109</v>
+      </c>
+      <c r="I25" s="91" t="s">
+        <v>43</v>
+      </c>
+      <c r="J25" s="4"/>
+      <c r="K25" s="4"/>
+      <c r="L25" s="4"/>
+    </row>
+    <row r="26" spans="1:12" s="92" customFormat="1" ht="63" x14ac:dyDescent="0.2">
+      <c r="A26" s="87" t="s">
+        <v>113</v>
+      </c>
+      <c r="B26" s="87" t="s">
+        <v>138</v>
+      </c>
+      <c r="C26" s="88" t="s">
+        <v>136</v>
+      </c>
+      <c r="D26" s="88" t="s">
+        <v>121</v>
+      </c>
+      <c r="E26" s="88" t="s">
+        <v>135</v>
+      </c>
+      <c r="F26" s="93"/>
+      <c r="G26" s="90" t="s">
+        <v>107</v>
+      </c>
+      <c r="H26" s="90" t="s">
+        <v>109</v>
+      </c>
+      <c r="I26" s="91" t="s">
+        <v>43</v>
+      </c>
+      <c r="J26" s="4"/>
+      <c r="K26" s="4"/>
+      <c r="L26" s="4"/>
+    </row>
+    <row r="27" spans="1:12" s="92" customFormat="1" ht="63" x14ac:dyDescent="0.2">
+      <c r="A27" s="87" t="s">
+        <v>114</v>
+      </c>
+      <c r="B27" s="87" t="s">
+        <v>139</v>
+      </c>
+      <c r="C27" s="88" t="s">
+        <v>137</v>
+      </c>
+      <c r="D27" s="88" t="s">
+        <v>121</v>
+      </c>
+      <c r="E27" s="88" t="s">
+        <v>135</v>
+      </c>
+      <c r="F27" s="93"/>
+      <c r="G27" s="90" t="s">
+        <v>107</v>
+      </c>
+      <c r="H27" s="90" t="s">
+        <v>109</v>
+      </c>
+      <c r="I27" s="91" t="s">
+        <v>43</v>
+      </c>
+      <c r="J27" s="4"/>
+      <c r="K27" s="4"/>
+      <c r="L27" s="4"/>
+    </row>
+    <row r="28" spans="1:12" s="92" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="A28" s="87"/>
+      <c r="B28" s="87"/>
+      <c r="C28" s="88"/>
+      <c r="D28" s="88"/>
+      <c r="E28" s="88"/>
+      <c r="F28" s="93"/>
+      <c r="G28" s="90"/>
+      <c r="H28" s="90"/>
+      <c r="I28" s="91"/>
+      <c r="J28" s="4"/>
+      <c r="K28" s="4"/>
+      <c r="L28" s="4"/>
+    </row>
+    <row r="29" spans="1:12" s="92" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="A29" s="87"/>
+      <c r="B29" s="87"/>
+      <c r="C29" s="88"/>
+      <c r="D29" s="88"/>
+      <c r="E29" s="88"/>
+      <c r="F29" s="93"/>
+      <c r="G29" s="90"/>
+      <c r="H29" s="90"/>
+      <c r="I29" s="91"/>
+      <c r="J29" s="4"/>
+      <c r="K29" s="4"/>
+      <c r="L29" s="4"/>
+    </row>
+    <row r="30" spans="1:12" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A30" s="73"/>
+      <c r="B30" s="73"/>
+      <c r="C30" s="74"/>
+      <c r="D30" s="74"/>
+      <c r="E30" s="74"/>
+      <c r="F30" s="75"/>
+      <c r="G30" s="76"/>
+      <c r="H30" s="76"/>
+      <c r="I30" s="77"/>
+      <c r="J30" s="75"/>
+      <c r="K30" s="75"/>
+      <c r="L30" s="75"/>
+    </row>
+    <row r="31" spans="1:12" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A31" s="73"/>
+      <c r="B31" s="73"/>
+      <c r="C31" s="74"/>
+      <c r="D31" s="74"/>
+      <c r="E31" s="74"/>
+      <c r="F31" s="75"/>
+      <c r="G31" s="76"/>
+      <c r="H31" s="76"/>
+      <c r="I31" s="77"/>
+      <c r="J31" s="42"/>
+      <c r="K31" s="42"/>
+      <c r="L31" s="42"/>
+    </row>
+    <row r="32" spans="1:12" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A32" s="73"/>
+      <c r="B32" s="73"/>
+      <c r="C32" s="74"/>
+      <c r="D32" s="74"/>
+      <c r="E32" s="74"/>
+      <c r="F32" s="75"/>
+      <c r="G32" s="76"/>
+      <c r="H32" s="76"/>
+      <c r="I32" s="77"/>
+      <c r="J32" s="42"/>
+      <c r="K32" s="42"/>
+      <c r="L32" s="42"/>
+    </row>
+    <row r="33" spans="1:12" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A33" s="73"/>
+      <c r="B33" s="73"/>
+      <c r="C33" s="74"/>
+      <c r="D33" s="74"/>
+      <c r="E33" s="74"/>
+      <c r="F33" s="78"/>
+      <c r="G33" s="76"/>
+      <c r="H33" s="76"/>
+      <c r="I33" s="79"/>
+      <c r="J33" s="42"/>
+      <c r="K33" s="42"/>
+      <c r="L33" s="42"/>
+    </row>
+    <row r="34" spans="1:12" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A34" s="42"/>
+      <c r="B34" s="42"/>
+      <c r="C34" s="42"/>
+      <c r="D34" s="42"/>
+      <c r="E34" s="42"/>
+      <c r="F34" s="42"/>
+      <c r="G34" s="42"/>
+      <c r="H34" s="42"/>
+      <c r="I34" s="42"/>
+      <c r="J34" s="42"/>
+      <c r="K34" s="42"/>
+      <c r="L34" s="42"/>
+    </row>
+    <row r="35" spans="1:12" ht="15" x14ac:dyDescent="0.2">
+      <c r="A35" s="32"/>
+      <c r="B35" s="32"/>
+      <c r="C35" s="32"/>
+      <c r="D35" s="32"/>
+      <c r="E35" s="32"/>
+      <c r="F35" s="33"/>
+      <c r="G35" s="32"/>
+      <c r="H35" s="32"/>
+      <c r="I35" s="32"/>
+      <c r="J35" s="32"/>
+      <c r="K35" s="32"/>
+      <c r="L35" s="32"/>
+    </row>
+    <row r="36" spans="1:12" ht="15" x14ac:dyDescent="0.2">
+      <c r="A36" s="94" t="s">
+        <v>5</v>
+      </c>
+      <c r="B36" s="32" t="s">
+        <v>111</v>
+      </c>
+      <c r="C36" s="32"/>
+      <c r="D36" s="32"/>
+      <c r="E36" s="32"/>
+      <c r="F36" s="33"/>
+      <c r="G36" s="32"/>
+      <c r="H36" s="32"/>
+      <c r="I36" s="32"/>
+      <c r="J36" s="32"/>
+      <c r="K36" s="32"/>
+      <c r="L36" s="32"/>
+    </row>
+    <row r="37" spans="1:12" ht="15" x14ac:dyDescent="0.2">
+      <c r="A37" s="95" t="s">
+        <v>6</v>
+      </c>
+      <c r="B37" s="48">
+        <v>43615</v>
+      </c>
+      <c r="C37" s="32"/>
+      <c r="D37" s="32"/>
+      <c r="E37" s="32"/>
+      <c r="F37" s="33"/>
+      <c r="G37" s="32"/>
+      <c r="H37" s="32"/>
+      <c r="I37" s="32"/>
+      <c r="J37" s="32"/>
+      <c r="K37" s="32"/>
+      <c r="L37" s="32"/>
+    </row>
+    <row r="38" spans="1:12" ht="15" x14ac:dyDescent="0.2">
+      <c r="A38" s="32"/>
+      <c r="B38" s="32"/>
+      <c r="C38" s="32"/>
+      <c r="D38" s="32"/>
+      <c r="E38" s="32"/>
+      <c r="F38" s="33"/>
+      <c r="G38" s="32"/>
+      <c r="H38" s="32"/>
+      <c r="I38" s="32"/>
+      <c r="J38" s="32"/>
+      <c r="K38" s="32"/>
+      <c r="L38" s="32"/>
+    </row>
+    <row r="39" spans="1:12" ht="15" x14ac:dyDescent="0.2">
+      <c r="A39" s="32"/>
+      <c r="B39" s="32"/>
+      <c r="C39" s="32"/>
+      <c r="D39" s="32"/>
+      <c r="E39" s="32"/>
+      <c r="F39" s="33"/>
+      <c r="G39" s="32"/>
+      <c r="H39" s="32"/>
+      <c r="I39" s="32"/>
+      <c r="J39" s="32"/>
+      <c r="K39" s="32"/>
+      <c r="L39" s="32"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="A18:C20"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3904,20 +5273,20 @@
     <row r="1" spans="1:6" s="17" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="1:6" s="17" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="65"/>
-      <c r="B2" s="119" t="s">
-        <v>45</v>
-      </c>
-      <c r="C2" s="120"/>
-      <c r="D2" s="120"/>
-      <c r="E2" s="120"/>
-      <c r="F2" s="121"/>
+      <c r="B2" s="131" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="132"/>
+      <c r="D2" s="132"/>
+      <c r="E2" s="132"/>
+      <c r="F2" s="133"/>
     </row>
     <row r="3" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="122"/>
-      <c r="C3" s="123"/>
-      <c r="D3" s="123"/>
-      <c r="E3" s="123"/>
-      <c r="F3" s="124"/>
+      <c r="B3" s="134"/>
+      <c r="C3" s="135"/>
+      <c r="D3" s="135"/>
+      <c r="E3" s="135"/>
+      <c r="F3" s="136"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B4" s="8"/>
@@ -3946,10 +5315,10 @@
         <v>1</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>80</v>
+        <v>128</v>
       </c>
       <c r="E6" s="20" t="s">
         <v>12</v>
@@ -3961,10 +5330,10 @@
         <v>2</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>82</v>
+        <v>129</v>
       </c>
       <c r="E7" s="20" t="s">
         <v>12</v>
@@ -3976,10 +5345,10 @@
         <v>3</v>
       </c>
       <c r="C8" s="19" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D8" s="19" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E8" s="20" t="s">
         <v>12</v>
@@ -3991,10 +5360,10 @@
         <v>4</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D9" s="19" t="s">
-        <v>84</v>
+        <v>130</v>
       </c>
       <c r="E9" s="20" t="s">
         <v>12</v>
@@ -4006,10 +5375,10 @@
         <v>5</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="E10" s="20" t="s">
         <v>12</v>
@@ -4021,10 +5390,10 @@
         <v>6</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="E11" s="20" t="s">
         <v>12</v>
@@ -4036,10 +5405,10 @@
         <v>7</v>
       </c>
       <c r="C12" s="19" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D12" s="19" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="E12" s="20" t="s">
         <v>12</v>
@@ -4051,10 +5420,10 @@
         <v>8</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D13" s="19" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="E13" s="20" t="s">
         <v>12</v>
@@ -4112,30 +5481,30 @@
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B22" s="14"/>
-      <c r="C22" s="125"/>
-      <c r="D22" s="125"/>
-      <c r="E22" s="125"/>
+      <c r="C22" s="137"/>
+      <c r="D22" s="137"/>
+      <c r="E22" s="137"/>
       <c r="F22" s="15"/>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B23" s="126" t="s">
+      <c r="B23" s="138" t="s">
         <v>13</v>
       </c>
       <c r="C23" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="D23" s="127"/>
-      <c r="E23" s="127"/>
-      <c r="F23" s="127"/>
+      <c r="D23" s="139"/>
+      <c r="E23" s="139"/>
+      <c r="F23" s="139"/>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B24" s="126"/>
+      <c r="B24" s="138"/>
       <c r="C24" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="D24" s="127"/>
-      <c r="E24" s="127"/>
-      <c r="F24" s="127"/>
+      <c r="D24" s="139"/>
+      <c r="E24" s="139"/>
+      <c r="F24" s="139"/>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B27" s="12"/>

</xml_diff>